<commit_message>
number separator product, debiturs, colls
</commit_message>
<xml_diff>
--- a/public/import/debitur/debitur.xlsx
+++ b/public/import/debitur/debitur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FC1C1E-98E3-45CD-9103-E842965681BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04F633-F3F3-4840-A5CE-9438043737C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD82610D-797C-4253-ACE6-E74E470448B8}"/>
   </bookViews>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1298A0-44C4-4729-B91A-A465C0FD90E6}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>